<commit_message>
Commit on 19-12-2024 after making changes required according to QA
</commit_message>
<xml_diff>
--- a/imy_se/Excel_Files/imy_se_sweden.xlsx
+++ b/imy_se/Excel_Files/imy_se_sweden.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="138">
   <si>
     <t>id</t>
   </si>
@@ -61,288 +61,267 @@
     <t>https://www.imy.se/en/news/unlawful-use-of-body-cams-in-stockholms-public-transport/</t>
   </si>
   <si>
+    <t>https://www.imy.se/en/news/administrative-fine-to-the-swedish-customs-for-deficient-routines/</t>
+  </si>
+  <si>
     <t>https://www.imy.se/en/news/swedish-authority-for-privacy-protection-issues-fine-against-the-national-government-service-centre/</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/news/administrative-fine-to-the-swedish-customs-for-deficient-routines/</t>
+    <t>https://www.imy.se/en/news/administrative-fine-of-sek-35-million-against-trygg-hansa/</t>
   </si>
   <si>
     <t>https://www.imy.se/en/news/gdpr-fine-for-unlawful-video-surveillance-in-an-lss-housing/</t>
   </si>
   <si>
+    <t>https://www.imy.se/en/news/the-swedish-data-protection-authority-imposes-administrative-fine-on-google/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/administrative-fine-against-region-uppsala-for-breaches-in-its-security/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/administrative-fine-against-klarna-after-investigation/</t>
+  </si>
+  <si>
     <t>https://www.imy.se/en/news/300000-sek-fine-against-housing-company/</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/news/administrative-fine-against-region-uppsala-for-breaches-in-its-security/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/administrative-fine-of-sek-35-million-against-trygg-hansa/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/the-swedish-data-protection-authority-imposes-administrative-fine-on-google/</t>
+    <t>https://www.imy.se/en/news/four-companies-must-stop-using-google-analytics/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/police-unlawfully-used-facial-recognition-app/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/wrongful-to-publish-sensitive-personal-data-on-region-orebro-countys-website/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/co-operative-housing-association-banned-from-using-video-surveillance-in-entrance-and-stairwell/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/administrative-fee-against-spotify/</t>
   </si>
   <si>
     <t>https://www.imy.se/en/news/fine-against-region-dalarna/</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/news/administrative-fine-against-klarna-after-investigation/</t>
+    <t>https://www.imy.se/en/news/hm-has-made-it-unnecessarily-difficult-to-avoid-marketing/</t>
   </si>
   <si>
     <t>https://www.imy.se/en/news/incorrect-use-of-247-surveillance-of-firefighters/</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/news/hm-has-made-it-unnecessarily-difficult-to-avoid-marketing/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/four-companies-must-stop-using-google-analytics/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/co-operative-housing-association-banned-from-using-video-surveillance-in-entrance-and-stairwell/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/police-unlawfully-used-facial-recognition-app/</t>
+    <t>https://www.imy.se/en/news/serious-deficiencies-in-the-stockholm-online-school-platform/</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/news/deficiencies-in-how-healthcare-providers-control-staff-access-to-patient-journal-data/</t>
   </si>
   <si>
     <t>https://www.imy.se/en/news/university-failed-to-sufficiently-protect-sensitive-personal-data/</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/news/administrative-fee-against-spotify/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/wrongful-to-publish-sensitive-personal-data-on-region-orebro-countys-website/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/deficiencies-in-how-healthcare-providers-control-staff-access-to-patient-journal-data/</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/news/serious-deficiencies-in-the-stockholm-online-school-platform/</t>
-  </si>
-  <si>
     <t>Unlawful use of body cams in Stockholm’s public transport</t>
   </si>
   <si>
+    <t>Administrative fine to the Swedish Customs for deficient routines</t>
+  </si>
+  <si>
     <t>Swedish Authority for Privacy Protection issues fine against the National Government Service Centre</t>
   </si>
   <si>
-    <t>Administrative fine to the Swedish Customs for deficient routines</t>
+    <t>Administrative fine of SEK 35 million against Trygg-Hansa</t>
   </si>
   <si>
     <t>GDPR fine for unlawful video surveillance in an LSS housing</t>
   </si>
   <si>
+    <t>Swedish Authority for Privacy Protection imposes administrative fine on Google</t>
+  </si>
+  <si>
+    <t>Administrative fine against Region Uppsala for breaches in its security</t>
+  </si>
+  <si>
+    <t>Administrative fine against Klarna after investigation</t>
+  </si>
+  <si>
     <t>300,000 SEK fine against housing company</t>
   </si>
   <si>
-    <t>Administrative fine against Region Uppsala for breaches in its security</t>
-  </si>
-  <si>
-    <t>Administrative fine of SEK 35 million against Trygg-Hansa</t>
-  </si>
-  <si>
-    <t>Swedish Authority for Privacy Protection imposes administrative fine on Google</t>
+    <t>Four companies must stop using Google Analytics</t>
+  </si>
+  <si>
+    <t>Police unlawfully used facial recognition app</t>
+  </si>
+  <si>
+    <t>Wrongful to publish sensitive personal data on Region Örebro County’s website</t>
+  </si>
+  <si>
+    <t>Co-operative housing association banned from using video surveillance in entrance and stairwel</t>
+  </si>
+  <si>
+    <t>Administrative fee against Spotify</t>
   </si>
   <si>
     <t>Fine against Region Dalarna</t>
   </si>
   <si>
-    <t>Administrative fine against Klarna after investigation</t>
+    <t>H&amp;M has made it unnecessarily difficult to avoid marketing</t>
   </si>
   <si>
     <t>Incorrect use of 24/7 surveillance of firefighters</t>
   </si>
   <si>
-    <t>H&amp;M has made it unnecessarily difficult to avoid marketing</t>
-  </si>
-  <si>
-    <t>Four companies must stop using Google Analytics</t>
-  </si>
-  <si>
-    <t>Co-operative housing association banned from using video surveillance in entrance and stairwel</t>
-  </si>
-  <si>
-    <t>Police unlawfully used facial recognition app</t>
+    <t>Serious deficiencies in the Stockholm online School Platform</t>
+  </si>
+  <si>
+    <t>Deficiencies in how healthcare providers control staff access to patient journal data</t>
   </si>
   <si>
     <t>University failed to sufficiently protect sensitive personal data</t>
   </si>
   <si>
-    <t>Administrative fee against Spotify</t>
-  </si>
-  <si>
-    <t>Wrongful to publish sensitive personal data on Region Örebro County’s website</t>
-  </si>
-  <si>
-    <t>Deficiencies in how healthcare providers control staff access to patient journal data</t>
-  </si>
-  <si>
-    <t>Serious deficiencies in the Stockholm online School Platform</t>
-  </si>
-  <si>
     <t>2021-07-13</t>
   </si>
   <si>
+    <t>2022-03-16</t>
+  </si>
+  <si>
     <t>2020-04-29</t>
   </si>
   <si>
-    <t>2022-03-16</t>
+    <t>2023-09-05</t>
   </si>
   <si>
     <t>2020-11-25</t>
   </si>
   <si>
+    <t>2020-03-11</t>
+  </si>
+  <si>
+    <t>2022-02-18</t>
+  </si>
+  <si>
+    <t>2022-03-31</t>
+  </si>
+  <si>
     <t>2020-12-15</t>
   </si>
   <si>
-    <t>2022-02-18</t>
-  </si>
-  <si>
-    <t>2023-09-05</t>
-  </si>
-  <si>
-    <t>2020-03-11</t>
+    <t>2023-07-03</t>
+  </si>
+  <si>
+    <t>2021-02-11</t>
+  </si>
+  <si>
+    <t>2020-05-12</t>
+  </si>
+  <si>
+    <t>2020-06-16</t>
+  </si>
+  <si>
+    <t>2023-06-13</t>
   </si>
   <si>
     <t>2023-01-24</t>
   </si>
   <si>
-    <t>2022-03-31</t>
-  </si>
-  <si>
     <t>2023-10-19</t>
   </si>
   <si>
-    <t>2023-07-03</t>
-  </si>
-  <si>
-    <t>2020-06-16</t>
-  </si>
-  <si>
-    <t>2021-02-11</t>
+    <t>2020-11-24</t>
+  </si>
+  <si>
+    <t>2020-12-03</t>
   </si>
   <si>
     <t>2020-12-11</t>
   </si>
   <si>
-    <t>2023-06-13</t>
-  </si>
-  <si>
-    <t>2020-05-12</t>
-  </si>
-  <si>
-    <t>2020-12-03</t>
-  </si>
-  <si>
-    <t>2020-11-24</t>
-  </si>
-  <si>
     <t>The Swedish Authority for Privacy Protection (IMY) concludes that SL, who operate the public transport in Stockholm, has violated GDPR when equipping ticket inspectors with body cameras that record video and sound. The IMY issues an administrative fine against SL of SEK 16 million. The IMY has investigated SL's use of body cameras. SL, who operates the public transport in Stockholm, has equipped ticket inspectors with body-worn cameras. The purpose of the cameras is to prevent threatening situations, to document incidents that have occurred and to ensure that the right person is fined for having travelled with public transport without a valid ticket. The ticket controllers' cameras continuously record images and sounds that are stored for one minute, after which the material is over-written unless the ticket inspector presses the record button on the camera. The ticket controllers are instructed to wear the camera during their entire work shift and can thus potentially film all travellers who pass the inspector. – In Stockholm's public transport, several hundred thousand people travel daily. This technology with continuous recording in practice means that a large number of travellers risk being monitored with both video and audio being recorded, says Jeanette Bladh Gustafson, lawyer at IMY's camera group. The IMY states that the technology with body-worn cameras can be used to prevent and document threatening situations, but that the time for pre-recording needs to be reduced to a maximum of 15 seconds. However, the authority does not consider that the technology can be used to confirm the identity of the person traveling without a valid ticket, where instead, for example, still images and no sound recording are sufficient. The IMY also criticizes the fact that SL has failed to adequately inform about the camera surveillance, for example that not only video but also sound is being recorded. – It is serious that SL does not inform about sound recordings because people using public transport in Stockholm cannot reasonably expect to have their conversations recorded. The different shortcomings combined regarding how SL uses body cameras leads the IMY to issue an administrative fine of SEK 16 million.</t>
   </si>
   <si>
+    <t>The Swedish Authority for Privacy Protection (IMY) has investigated a personal data breach within the Swedish Customs and notes that the agency has had deficient routines and insufficient technical barriers, which has led to data from criminal investigations being transferred from staff mobile phones to a US cloud service. IMY has now completed an investigation of a personal data breach at the Swedish Customs. A couple of employees at the Swedish Customs' law enforcement activities have used the cloud service Google Photo in their staff mobile phones. The officials had linked their private Google Photo accounts to their mobile phones, which automatically synced the photos and videos taken in their official duty to the cloud service. The Swedish Customs has stated that the use of Google Photos was not permitted within the authority. “The fact that the use of the cloud service was unauthorized does not deprive the Swedish Customs of the responsibility that the authority has as data controller. The Swedish Customs has not taken appropriate technical and organizational measures to prevent what happened. Existing routines and technical barriers to prevent data from staff mobiles being copied and stored in a US cloud service were insufficient”, says Jonas Agnvall who led the investigation. IMY's decision states, among other things, that there needs to be clear routines and guidelines for employees' use of company mobiles and that employees also need to receive training and information on how personal data may be processed on the mobile phones. “There should also be technical restrictions for which apps that can be downloaded to the staff mobiles.” However, IMY notes that there are also mitigating circumstances. There have only been a few employees who have used the cloud service without the authority's approval. Images and movies uploaded to the cloud service have been deleted. In addition, after the incident was discovered, the Swedish Customs has taken both technical and organizational measures to prevent similar incidents, among other things by clarifying guidelines and limiting the possibilities of downloading applications. “We issue an administrative fine of SEK 300,000 against the Swedish Customs, which is a considerably lower amount than what would have been justified without the mitigating circumstances”, says Jonas Agnvall.</t>
+  </si>
+  <si>
     <t>Swedish Authority for Privacy Protection imposes an administrative fine of 200 000 Swedish kronor (approximately 18 700 euro) on the National Government Service Centre for failing to notify affected parties as well as the Data Protection Authority about a personal data breach in due time Swedish Authority for Privacy Protection (DPA) initiated an investigation against the National Government Service Centre (NGSC) upon having received a number of personal data breach notifications concerning an error in the IT system for salary administration. The error entailed the possibility of unauthorised access to personal data of both personnel of authorities using the system and of the personnel of the NGSC. - Our investigation shows that it has taken too long for the NGSC to inform the concerned parties about the error and furthermore that the NGSC has failed to report the personal data breach to the DPA in due time. The documentation of the breach, as required under the GDPR, was also found incomplete with regards to the NGSC’s personnel and their data, says Elin Hallström, legal advisor, who has been leading the DPA’s audit. The DPA noted that it took almost five months for the NGSC to notify the concerned parties and close to three months before the DPA received a data breach notification. - When a data breach of this kind is discovered by a processor such as the NGSC in this case, it is important to inform the controllers as soon as possible so that they can report the breach to the DPA and take further actions to mitigate any related risks. The NGSC has failed to act in time. In its decision the DPA orders the NGSC to introduce internal routines for the documentation of personal data breaches and to verify that those routines are abided by. Together with this order the DPA imposes an administrative fine on the NGSC of in total 200 000 Swedish kronor. The National Government Service Centre coordinates the administration of government agencies by offering administrative support services to other government agencies. It offers basic services in the areas of salary administration, financial administration and eCommerce.</t>
   </si>
   <si>
-    <t>The Swedish Authority for Privacy Protection (IMY) has investigated a personal data breach within the Swedish Customs and notes that the agency has had deficient routines and insufficient technical barriers, which has led to data from criminal investigations being transferred from staff mobile phones to a US cloud service. IMY has now completed an investigation of a personal data breach at the Swedish Customs. A couple of employees at the Swedish Customs' law enforcement activities have used the cloud service Google Photo in their staff mobile phones. The officials had linked their private Google Photo accounts to their mobile phones, which automatically synced the photos and videos taken in their official duty to the cloud service. The Swedish Customs has stated that the use of Google Photos was not permitted within the authority. “The fact that the use of the cloud service was unauthorized does not deprive the Swedish Customs of the responsibility that the authority has as data controller. The Swedish Customs has not taken appropriate technical and organizational measures to prevent what happened. Existing routines and technical barriers to prevent data from staff mobiles being copied and stored in a US cloud service were insufficient”, says Jonas Agnvall who led the investigation. IMY's decision states, among other things, that there needs to be clear routines and guidelines for employees' use of company mobiles and that employees also need to receive training and information on how personal data may be processed on the mobile phones. “There should also be technical restrictions for which apps that can be downloaded to the staff mobiles.” However, IMY notes that there are also mitigating circumstances. There have only been a few employees who have used the cloud service without the authority's approval. Images and movies uploaded to the cloud service have been deleted. In addition, after the incident was discovered, the Swedish Customs has taken both technical and organizational measures to prevent similar incidents, among other things by clarifying guidelines and limiting the possibilities of downloading applications. “We issue an administrative fine of SEK 300,000 against the Swedish Customs, which is a considerably lower amount than what would have been justified without the mitigating circumstances”, says Jonas Agnvall.</t>
+    <t>Trygg-Hansa's security flaws have meant that information about 650,000 customers has been accessible to unauthorized persons via the internet. The Swedish Authority for Privacy Protection (IMY) is now issuing an administrative fine of SEK 35 million against the company. After receiving a tip, IMY started an investigation of the insurance company Trygg-Hansa (then Moderna Försäkringar). The person who contacted IMY had received an email from the company with a link to a web page with price quotes. On this web page, there were clickable links with URLs that led to documents with insurance information. However, the person noticed that it was possible to access other policyholders' documents, without any kind of login, by simply replacing a few numbers in the web link. – The documents that have been accessible to unauthorized persons have in some cases contained sensitive personal data, including information about health that also had a high level of detail, so that it was possible to find out, for example, how a health problem arose or details about a health condition. All in all, the large amount of personal data has made it possible to create a clear picture of a person's private circumstances, says Evelin Palmér, legal advisor at IMY. Possible to access data for more than two years IMY's supervision has shown that it was possible to access customer data for 650,000 customers during the period October 2018 to February 2021. Among the customer data, in addition to data on health, there is also other data such as financial information, contact details, social security numbers and insurance holdings. In its decision, IMY states that the deficiencies have been of such a fundamental nature that Trygg-Hansa should have had the opportunity to discover and remedy these even before the relevant IT system was introduced and in any case during the long period that the system was used. IMY concludes that Trygg-Hansa has not taken appropriate technical measures to ensure a level of security that is appropriate in relation to the risk. The authority therefore issues an administrative fine of SEK 35 million against the company. Clarification The security deficiency that IMY has found in the current case was at the insurance company Moderna Försäkringar. IMY clarifies that Moderna Försäkringar has subsequently, in April 2022, merged with Trygg-Hansa and in connection with that changed its name to Trygg-Hansa.</t>
   </si>
   <si>
     <t>Swedish Authority for Privacy Protection issues an administrative fine of SEK 200,000 against Gnosjö Municipality for unlawful video surveillance in an LSS housing. Swedish Authority for Privacy Protection received a complaint from a relative of a resident of a residential care home for persons with certain functional impairments (so-called LSS housing) in Gnosjö municipality, claiming that the resident was being monitored illegally. The Authority initiated an audit of the LSS housing and can conclude that the resident in question indeed was monitored in their bedroom in violation of the General Data Protection Regulation, GDPR, and the Swedish Video Surveillance Act. "The resident has been monitored in the most private sphere of the home, which led to a severe and unjustifiable interference with the residents' right to privacy" says Jeanette Bladh Gustafson, lawyer at Swedish Authority for Privacy Protection's unit for video surveillance. The Social Welfare Committee in Gnosjö, which is responsible for the LSS housing, has stated that the resident's disease profile has created major difficulties both for the resident himself and for the staff, and that situations have arisen where there has been a risk to the life and health of the resident. There has also been situations where the staff has suffered injuries. Swedish Authority for Privacy Protection shares the assessment of the Social Committee that there has been a need to take measures to manage and improve the situation. — However, it should be possible for the LSS housing to achieve the same purposes as those for which the video surveillance was carried out with less privacy-intrusive means. Swedish Authority for Privacy Protection concludes in its decision that there is no legal basis for the video surveillance, that an impact assessment has not been carried out before initiating the video surveillance and that the controller has failed to clearly inform about the video surveillance. For those reasons, Swedish Authority for Privacy Protection issues an administrative fine of SEK 200,000 against the Social Welfare Committee.</t>
   </si>
   <si>
+    <t>Swedish Authority for Privacy Protection imposes a fine of 75 million Swedish kronor (approximately 7 million euro) on Google for failure to comply with the GDPR. Google as a search engine operator has not fulfilled its obligations in respect of the right to request delisting In 2017 Swedish Authority for Privacy Protection (DPA) finalised an audit concerning how Google handles individuals’ right to have search result listings for searches that includes their name removed from Google’s search engine in case of for example lack of accuracy, relevance or if considered superfluous. In its decision the DPA concluded that a number of search result listings should be removed and subsequently ordered Google to do so. In 2018, due to indications that Google had not fully complied with the previously issued order, the DPA initiated a follow-up audit. This audit is now finalised and the DPA is issuing a fine against Google. – The General Data Protection Regulation, GDPR, increases the level of responsibility for organisations that collect and process personal data, and strengthens the rights of individuals. An important part of those rights is the possibility for individuals to have their search result delisted. We have found that Google is not fully complying with its obligations in relation to this data protection right, says Lena Lindgren Schelin, Director General at the Swedish DPA. Swedish Authority for Privacy Protection is critical to the fact that Google did not properly remove two of the search result listings that the DPA had ordered them to remove back in 2017. In one of the cases Google has done a too narrow interpretation of what web addresses needed to be removed from the search result listing. In the second case Google has failed to remove the search result listing without undue delay. When Google removes a search result listing, it notifies the website to which the link is directed in a way that gives the site-owner knowledge of which webpage link was removed and who was behind the delisting request. This allows the site-owner to re-publish the webpage in question on another web address that will then be displayed in a Google search. This in practice puts the right to delisting out of effect. – In its delisting request form Google states that the site-owner will be notified of the request in a way that might result in individuals refraining from exercising their right to request delisting, thereby undermining the effectiveness of this right, says Olle Pettersson, legal advisor at the Swedish DPA who has participated in this audit of Google. Google does not have a legal basis for informing site-owners when search result listings are removed and furthermore gives individuals misleading information by the statement in the request form. That is why the DPA orders Google to cease and desist from this practice. Facts about the right to have search result listings removed In May 2014 the Court of Justice of the EU ruled that an individual may request a search engine provider such as Google to remove a search result listing that contains the name of an individual in case the listing is incorrect, irrelevant or superfluous. This right was strengthened with the GDPR entering into force 25th May 2018. The right is however not absolute, you cannot demand that all search results are to be removed. Individuals who wish to exercise their right to request delisting should contact the search engine provider directly. What happens next? Google may appeal the decision of the Swedish DPA within three weeks. If Google decides not to appeal, the decision will enter into force by the end of that time period. Once the decision has entered into force it will be handed over to the Legal, Financial and Administrative Services Agency (Kammarkollegiet) that handles the administration of fines under the GDPR.</t>
+  </si>
+  <si>
+    <t>IMY issues an administrative fine of in total SEK 1.9 million against Region Uppsala after finding that the region has not taken appropriate security measures in its handling of sensitive personal data. The Swedish Authority for Privacy Protection (IMY) has received two personal data breach notifications from Region Uppsala. The data breaches concern sensitive personal data sent without encryption to recipients in and outside Sweden. Following the data breach notifications, IMY has initiated investigations of the region (both the regional board and the hospital board) and states in its two decisions that the region has not taken sufficient technical and organizational measures to ensure a security level that is appropriate in relation to the risks involved in the personal data processing. “It is a question of information about health and thus sensitive personal information. Our supervision show that sufficient technical security measures have not been taken to protect the data against, for example, unauthorized access. They also show that the processing of personal data in both cases took place in violation of the region's own guidelines, which also indicates shortcomings in the organizational measures”, says Linda Hamidi, who led the investigations. One of the investigations concerns sensitive personal data and social security numbers sent via e-mail. The actual transmission of the e-mail was encrypted but not the information in the e-mails. This concerns e-mails with patient data that have been sent automatically to the relevant healthcare administrations within the region, and partly e-mails with patient data that have been sent manually to researchers and doctors within the region. For the identified shortcomings in this investigation, IMY issues an administrative fine of SEK 300,000 against the regional board of the Uppsala Region. The second investigation concerns how the University Hospital in Uppsala sends e-mails with patient data to patients and referrers in third countries, i.e. countries outside the EU. The supervision also covers the storage of patient data in the hospital's e-mail server. IMY has examined the security of the personal data processed but has not examined the legality of the third-country transfer itself. For the identified shortcomings in this investigation, IMY issues an administrative fine of SEK 1.6 million against the hospital board in the Uppsala Region. Taken together, the two investigations show that the region has not taken the necessary measures to protect sensitive personal data in the e-mails sent and in the storage of the data in the hospital's e-mail server.</t>
+  </si>
+  <si>
+    <t>The Swedish Authority for Privacy Protection (IMY) issues an administrative fine of SEK 7,500,000 against Klarna Bank AB after an investigation has shown that the company has not complied with several of the rules in the GDPR. IMY has now finished an investigation of Klarna Bank AB (Klarna). The authority has examined how the company on its website informs about how it processes personal data in accordance with the GDPR. – Klarna is a financial company that processes personal data about many people and in many different ways. It is important that the information that Klarna provides about how the company processes personal data is correct and as complete as possible. Here we have seen shortcomings, says lawyer Hans Kärnlöf who led the investigation. During the investigation, Klarna has continuously changed the information provided on how the company handles personal data. IMY's decision concerns the information provided in the spring of 2020. In its decision, IMY states that Klarna did not then provide information on the purpose for which and on the basis of which legal basis personal data was processed in one of the company's services. The company also provided incomplete and misleading information about who were the recipients of different categories of personal data when data was shared with Swedish and foreign credit information companies. Klarna also did not provide information on to which countries outside the EU/EEA personal data were transferred or on where and how individuals could obtain information on the safeguards that applied to the transfer to third countries. IMY also notes that the company provided incomplete information about the data subjects' rights, including the right to delete data, the right to data portability and the right to object to how one's personal data is processed. IMY issues an administrative fine against Klarna of SEK 7,500,000 for the deficiencies discovered during the investigation.</t>
+  </si>
+  <si>
     <t>Swedish Authority for Privacy Protection has issued an administrative fine of SEK 300,000 against a housing company for unlawful video surveillance in an apartment building. Swedish Authority for Privacy Protection (DPA) received a complaint concerning video surveillance in an apartment building belonging to the housing company Uppsalahem. The complainant claimed that there was a surveillance camera in the apartment house directed towards the complainant's front door. The DPA's audit shows that the housing company had set up a surveillance camera monitoring the floor where the complainant lives. The camera's monitoring area clearly covered two apartment doors, one of which belongs to the complainant and the other belonging to a resident whom has been subject to disturbances and harassment. The housing company states that the purpose of the video surveillance was to resolve disturbances having occurred in the stairwell over time. "The way the video surveillance was set up, on the ground floor of the property, left all residents of the house subject to monitoring on their way to and from their respective home. This is especially true for the complainant and the closest neighbour, since their front doors are so clearly included in the monitoring area of the video surveillance. Even if the company had a legitimate interest for video surveillance, it was outweighed by the residents' right to privacy," says Gustav Linder, legal advisor at Swedish Authority for Privacy Protection's video surveillance team. In its decision, Swedish Authority for Privacy Protection concludes that the video surveillance in question, monitoring individuals in their home environment is particularly privacy sensitive. For that reason, the DPA imposes a fine of SEK 300,000 on the housing company. The housing company has ceased the video surveillance in question.</t>
   </si>
   <si>
-    <t>IMY issues an administrative fine of in total SEK 1.9 million against Region Uppsala after finding that the region has not taken appropriate security measures in its handling of sensitive personal data. The Swedish Authority for Privacy Protection (IMY) has received two personal data breach notifications from Region Uppsala. The data breaches concern sensitive personal data sent without encryption to recipients in and outside Sweden. Following the data breach notifications, IMY has initiated investigations of the region (both the regional board and the hospital board) and states in its two decisions that the region has not taken sufficient technical and organizational measures to ensure a security level that is appropriate in relation to the risks involved in the personal data processing. “It is a question of information about health and thus sensitive personal information. Our supervision show that sufficient technical security measures have not been taken to protect the data against, for example, unauthorized access. They also show that the processing of personal data in both cases took place in violation of the region's own guidelines, which also indicates shortcomings in the organizational measures”, says Linda Hamidi, who led the investigations. One of the investigations concerns sensitive personal data and social security numbers sent via e-mail. The actual transmission of the e-mail was encrypted but not the information in the e-mails. This concerns e-mails with patient data that have been sent automatically to the relevant healthcare administrations within the region, and partly e-mails with patient data that have been sent manually to researchers and doctors within the region. For the identified shortcomings in this investigation, IMY issues an administrative fine of SEK 300,000 against the regional board of the Uppsala Region. The second investigation concerns how the University Hospital in Uppsala sends e-mails with patient data to patients and referrers in third countries, i.e. countries outside the EU. The supervision also covers the storage of patient data in the hospital's e-mail server. IMY has examined the security of the personal data processed but has not examined the legality of the third-country transfer itself. For the identified shortcomings in this investigation, IMY issues an administrative fine of SEK 1.6 million against the hospital board in the Uppsala Region. Taken together, the two investigations show that the region has not taken the necessary measures to protect sensitive personal data in the e-mails sent and in the storage of the data in the hospital's e-mail server.</t>
-  </si>
-  <si>
-    <t>Trygg-Hansa's security flaws have meant that information about 650,000 customers has been accessible to unauthorized persons via the internet. The Swedish Authority for Privacy Protection (IMY) is now issuing an administrative fine of SEK 35 million against the company. After receiving a tip, IMY started an investigation of the insurance company Trygg-Hansa (then Moderna Försäkringar). The person who contacted IMY had received an email from the company with a link to a web page with price quotes. On this web page, there were clickable links with URLs that led to documents with insurance information. However, the person noticed that it was possible to access other policyholders' documents, without any kind of login, by simply replacing a few numbers in the web link. – The documents that have been accessible to unauthorized persons have in some cases contained sensitive personal data, including information about health that also had a high level of detail, so that it was possible to find out, for example, how a health problem arose or details about a health condition. All in all, the large amount of personal data has made it possible to create a clear picture of a person's private circumstances, says Evelin Palmér, legal advisor at IMY. IMY's supervision has shown that it was possible to access customer data for 650,000 customers during the period October 2018 to February 2021. Among the customer data, in addition to data on health, there is also other data such as financial information, contact details, social security numbers and insurance holdings. In its decision, IMY states that the deficiencies have been of such a fundamental nature that Trygg-Hansa should have had the opportunity to discover and remedy these even before the relevant IT system was introduced and in any case during the long period that the system was used. IMY concludes that Trygg-Hansa has not taken appropriate technical measures to ensure a level of security that is appropriate in relation to the risk. The authority therefore issues an administrative fine of SEK 35 million against the company. The security deficiency that IMY has found in the current case was at the insurance company Moderna Försäkringar. IMY clarifies that Moderna Försäkringar has subsequently, in April 2022, merged with Trygg-Hansa and in connection with that changed its name to Trygg-Hansa.</t>
-  </si>
-  <si>
-    <t>Swedish Authority for Privacy Protection imposes a fine of 75 million Swedish kronor (approximately 7 million euro) on Google for failure to comply with the GDPR. Google as a search engine operator has not fulfilled its obligations in respect of the right to request delisting In 2017 Swedish Authority for Privacy Protection (DPA) finalised an audit concerning how Google handles individuals’ right to have search result listings for searches that includes their name removed from Google’s search engine in case of for example lack of accuracy, relevance or if considered superfluous. In its decision the DPA concluded that a number of search result listings should be removed and subsequently ordered Google to do so. In 2018, due to indications that Google had not fully complied with the previously issued order, the DPA initiated a follow-up audit. This audit is now finalised and the DPA is issuing a fine against Google. – The General Data Protection Regulation, GDPR, increases the level of responsibility for organisations that collect and process personal data, and strengthens the rights of individuals. An important part of those rights is the possibility for individuals to have their search result delisted. We have found that Google is not fully complying with its obligations in relation to this data protection right, says Lena Lindgren Schelin, Director General at the Swedish DPA. Swedish Authority for Privacy Protection is critical to the fact that Google did not properly remove two of the search result listings that the DPA had ordered them to remove back in 2017. In one of the cases Google has done a too narrow interpretation of what web addresses needed to be removed from the search result listing. In the second case Google has failed to remove the search result listing without undue delay. When Google removes a search result listing, it notifies the website to which the link is directed in a way that gives the site-owner knowledge of which webpage link was removed and who was behind the delisting request. This allows the site-owner to re-publish the webpage in question on another web address that will then be displayed in a Google search. This in practice puts the right to delisting out of effect. – In its delisting request form Google states that the site-owner will be notified of the request in a way that might result in individuals refraining from exercising their right to request delisting, thereby undermining the effectiveness of this right, says Olle Pettersson, legal advisor at the Swedish DPA who has participated in this audit of Google. Google does not have a legal basis for informing site-owners when search result listings are removed and furthermore gives individuals misleading information by the statement in the request form. That is why the DPA orders Google to cease and desist from this practice. In May 2014 the Court of Justice of the EU ruled that an individual may request a search engine provider such as Google to remove a search result listing that contains the name of an individual in case the listing is incorrect, irrelevant or superfluous. This right was strengthened with the GDPR entering into force 25th May 2018. The right is however not absolute, you cannot demand that all search results are to be removed. Individuals who wish to exercise their right to request delisting should contact the search engine provider directly. Google may appeal the decision of the Swedish DPA within three weeks. If Google decides not to appeal, the decision will enter into force by the end of that time period. Once the decision has entered into force it will be handed over to the Legal, Financial and Administrative Services Agency (Kammarkollegiet) that handles the administration of fines under the GDPR.</t>
+    <t>The Swedish Authority for Privacy Protection (IMY) has audited how four companies use Google Analytics for web statistics. IMY issues administrative fines against two of the companies. One of the companies has recently stopped using the statistics tool on its own initiative, while IMY orders the other three to also stop using it. IMY has audited how four companies transfer personal data to the US via Google Analytics, which is a tool for measuring and analysing traffic on websites. The companies audited are CDON, Coop, Dagens Industri and Tele2. The audits concerns a version of Google Analytics from 14th of August 2020. The audits are based on complaints from the organisation None of Your Business (NOYB) in the light of the Schrems II ruling by the European Court of Justice (CJEU). The complaints allege that the companies, in violation of the law, transfer personal data to the United States. According to the data protection regulation, GDPR, personal data may be transferred to third countries, i.e. countries outside the EU/EEA, if the European Commission has decided that the country in question has an adequate level of protection for personal data that corresponds to that within the EU/EEA. However, the CJEU ruled through the Schrems II ruling that the United States could not be considered to have such an adequate level of protection at the time of the ruling. In its audits, IMY considers that the data transferred to the US via Google's statistics tool is personal data because the data can be linked with other unique data that is transferred. The authority also concludes that the technical security measures that the companies have taken are not sufficient to ensure a level of protection that essentially corresponds to that guaranteed within the EU/EEA. – By the fact that IMY has decided on these cases at the same time, it is made clear what requirements are placed on technical security measures and other measures when transferring personal data to a third country, in this case the United States, says legal advisor Sandra Arvidsson, who led the audits of the companies. If there is no decision on an adequate level of protection by the European Commission, data may be transferred based on standard contractual clauses that the European Commission has decided on. However, according to the CJEU, such standard contractual clauses may need to be supplemented with additional safeguards if it is necessary for the protection that the clauses are intended to provide to be maintained in practice. All four companies have based their decisions on the transfer of personal data via Google Analytics on standard contractual clauses. From IMY's audits, it appears that none of the companies' additional technical security measures are sufficient. IMY issues an administrative fine of 12 million SEK against Tele2 and 300,000 SEK against CDON, which has not taken the same extensive protective measures as Coop and Dagens Industri. Tele2 has recently stopped using the statistics tool on its own initiative. IMY orders the other three companies to stop using the tool. – These decisions have implications not only for these four companies, but can also provide guidance for other organisations that use Google Analytics, says Sandra Arvidsson. The decisions For more information contact Legal advisor Sandra Arvidsson, telephone 08-515 154 14 Press service, telephone 08-515 15 415</t>
+  </si>
+  <si>
+    <t>The Swedish Authority for Privacy Protection finds that the Swedish Police Authority has processed personal data in breach of the Swedish Criminal Data Act when using Clearview AI to identify individuals. Upon news in the media of the Swedish Police Authority using the application Clearview AI for facial recognition the Swedish Authority for Privacy Protection (IMY) initiated an investigation against the Police. The investigation concludes that Cleaview AI has been used by the Police on a number of occasions. According to the Police a few employees have used the application without any prior authorisation. IMY concludes that the Police has not fulfilled its obligations as a data controller on a number of accounts with regards to the use of Clearview AI. The Police has failed to implement sufficient organisational measures to ensure and be able to demonstrate that the processing of personal data in this case has been carried out in compliance with the Criminal Data Act. When using Clearview AI the Police has unlawfully processed biometric data for facial recognition as well as having failed to conduct a data protection impact assessment which this case of processing would require. – There are clearly defined rules and regulations on how the Police Authority may process personal data, especially for law enforcement purposes. It is the responsibility of the Police to ensure that employees are aware of those rules, says Elena Mazzotti Pallard, legal advisor at IMY. IMY imposes an administrative fine of SEK 2,500,000 (approximately EUR 250,000) on the Police Authority for infringements of the Criminal Data Act. IMY also orders the Police to conduct further training and education of its employees in order to avoid any future processing of personal data in breach of data protection rules and regulations. In addition the Police is ordered to inform the data subjects, whose data has been disclosed to Clearview AI, when confidentiality rules so allows. Finally the Police are ordered to ensure, to the extent possible, that any personal data transferred to Clearview AI is erased.</t>
+  </si>
+  <si>
+    <t>Swedish Authority for Privacy Protection’s investigation shows that the Healthcare Committee in Region Örebro County made a mistake when publishing on the region’s website sensitive personal data about a patient admitted to a forensic psychiatric clinic. Swedish Authority for Privacy Protection received a complaint against the Healthcare Committee in Region Örebro County, in which claims that sensitive personal data about a patient admitted to forensic psychiatry clinic had been published on the region’s website was put forward. – Our investigation into the matter shows that sensitive personal data has wrongfully been published and thereby made accessible to the public on the region’s website", says Elin Hallström, Legal Advisor at Swedish Authority for Privacy Protection. Swedish Authority for Privacy Protection’s audit shows that there are no written instructions relating to the publication of documents and personal data on the website in place. Instructions for publishing information are instead communicated orally. In this case, the instructions had not been followed which led to the accidental publication of the document, suggesting that the Committee had not taken sufficient organizational measures to ensure that personal data is protected from being wrongfully published on the region’s website. – For this reason, we are now ordering the Committee to establish written instructions and introduce measures that ensure that those who publishes personal data on the region’s website does so in accordance with set instructions. In its decision, Swedish Authority for Privacy Protection also concludes that in terms of publication the Committee had neither a legitimate purpose, nor a legal basis, nor fulfilled the requirements for an exemption from the general prohibition against handling sensitive personal data in the General Data Protection Regulation. Swedish Authority for Privacy Protection orders the Committee to bring its personal data handling into compliance and furthermore issues an administrative fine of 120 000 Swedish kronor (approx. 11 000 euro) against the Committee. The published document in question has been removed from the region’s website.</t>
+  </si>
+  <si>
+    <t>Swedish Authority for Privacy Protection (DPA) has investigated a co-operative housing association’s use of video surveillance on its property. The DPA concludes that the association has gone too far when using video surveillance in the main entrance and the stairwell and when recording audio. The Swedish DPA has received complaints claiming that a co-operative housing association monitors the stairwell in the association's apartment building. The DPA has now finished an audit of the association. Swedish Authority for Privacy Protection's investigation shows that the association has four surveillance cameras installed. Two are located in the stairwell, one in the main entrance and one is directed towards a distribution box in the association's storage room. All cameras record video and audio non-stop 24 hrs 7 days a week. For the two cameras set up in the stairwell, Swedish Authority for Privacy Protection notes that these allow the association to map the habits, visits and social circle of the residents. "Already the fact that the surveillance is of the residents and their home environment means that it requires very strong reasons for the monitoring to be allowed," writes the authority in its decision. – Under special circumstances, a co-operative housing association may monitor a stairwell. However, in order for such surveillance to be allowed, the association must be able to demonstrate a pressing need for such video surveillance and that has not been the case here, says Nils Henckel, legal advisor at the Swedish DPA. The third camera is set up at the main entrance and the association states that it is to combat problems with vandalism, which it had experienced during two months in 2018. The Swedish DPA stresses the obligation to continuously review whether a need for video surveillance is justified and concludes that no such need was still present to date. As for the fourth camera, which is directed towards the distribution box, the DPA concludes that it must be re-directed so that it does not monitor the residents' storage facilities. Furthermore, Swedish Authority for Privacy Protection notes that audio recording constitutes an additional intrusion into the private sphere, in particular when recorded in a residential building, and that there are no circumstances that motivates such intrusion in this case. The Swedish DPA also concludes that the association has failed to properly inform the residents about the video surveillance. That includes the lack of information about the data controller, where to turn to for further detailed information and that audio is recorded, which is a particularly severe omission. Swedish Authority for Privacy Protection orders the co-operative housing association to stop the video surveillance of the stairwell and entrance, to cease audio recording for the surveillance camera by the distribution box and to improve the information provided concerning the video surveillance. Swedish Authority for Privacy Protection furthermore issues an administrative fine of 20 000 Swedish kronor (approximately 2 000 euro) against the association. When calculating the amount of the fine, consideration was taken to the fact that it was a smaller co-operative housing association</t>
+  </si>
+  <si>
+    <t>The Swedish Authority for Privacy Protection (IMY) has audited how Spotify handles customers' right to access their personal data. The deficiencies that have been discovered cause IMY to issue an administrative fine of SEK 58 million against the company. The General Data Protection Regulation, GDPR, entered into force in 2018 and means, among other things, that the rights of individuals are strengthened. One such right is the right of access, which means a right for individuals to find out what personal data a business handles about the person in question and to receive information about how this data is used. IMY has audited how Spotify handles the right for individuals to access their personal data. IMY assesses that Spotify releases the personal data the company processes when individuals request it, but that the company does not inform clearly enough about how this data is used by the company. - The information that the company provides about how and for what purposes individuals' personal data is handled should be more specific. It must be easy for the person requesting access to their data to understand how the company uses this data. In addition, personal data that is difficult to understand, such as those of a technical nature, may need to be explained not only in English but in the individual's own, native language. In these parts, we have seen certain shortcomings, says Karin Ekström, who is one of the legal advisors who led the supervision. Customers who have turned to Spotify to request access to their personal data have been able to choose which personal data they want access to because Spotify has divided the customers' personal data into different layers. One layer contains the information that Spotify has deemed to be of greatest interest to the individual, for example the customer's contact and payment details, which artists the customer follows and listening history for a certain period of time. If the customer wants more detailed information, for example all technical log files relating to the customer, it has also been possible to request these in another layer. - There is no obstacle to dividing the copy of personal data into different layers as long as the right to access is satisfied. In some situations, on the contrary, it can make it easier for the data subject to take in the information if it is presented in different parts, at least when it is a question of an extensive amount of information. It is important that the individual understands what information is in the various layers and how it can be requested. Here we believe that Spotify has done enough, says Karin Ekström. The purpose of the right of access is to give individuals the opportunity to check that the processing of their personal data is lawful. That the individual receives sufficient information is often a prerequisite for exercising other rights, for example the right to have incorrect information corrected or removed. As the information provided by Spotify has been unclear, it has been difficult for individuals to understand how their personal data is processed and to check whether the handling of their personal data is lawful. Spotify has taken several measures with the aim of meeting the requirements for individuals' right to access, and the deficiencies that have been discovered are considered overall to be of a low level of seriousness. In light of that and, among other things, the number of registered users and Spotify's turnover, IMY issues an administrative fine of SEK 58 million against Spotify for not having provided sufficiently clear information to individuals. Since Spotify has users in many countries, this decision has been made in cooperation with other data protection authorities in the EU.</t>
   </si>
   <si>
     <t>The Swedish Supervisory Authority issues an administrative fine against Region Dalarna which had sent appointment letters by mail to patients with sensitive personal data visible in window envelopes. The Swedish SA has initiated an audit of Region Dalarna after receiving complaints that the region had printed appointment letters to patients where the healthcare facility to which the visit refers was fully visible in the window envelope. The Swedish DPA has concluded that the processing of personal data in the current case is partially automated and that the data protection regulation is applicable. The use of window envelopes when sending appointment letters from the clinics covered by the audit, where the current care facility was visible in the window envelope, means that sensitive personal data has been disclosed without authorization for an unknown number of people who came into contact with the letter. This refers to about 2,500 letters per year, including to a children's and youth medicine clinic and a therapy clinic for children and young people. – This means that sensitive personal data about the patient has been available to, for example, the person who delivers the mail, the person who lives with the recipient and the person who received a letter that was delivered to the wrong address. The data has therefore not been adequately protected, says legal advisor Maja Welander, who led the audit. The health care board in Region Dalarna states that it has procured a service for sending appointment letters where it should not be clear from the envelope which clinic a letter regarding a healthcare visit refers to. After IMY began its audit, however, the board carried out an investigation which showed that the service in question did not cover all appointment lettersand that letters from certain care facilities were therefore sent in envelopes showing which clinic the visit referred to. The Swedish DPA states in its decision that the region has not taken sufficient security measures to protect sensitive personal data against unauthorized disclosure in connection with the sending of physical invitations to certain healthcare visits within the region. The authority therefore issues an administrative sanction of SEK 200,000 against the region for breach of the data protection regulation.</t>
   </si>
   <si>
-    <t>The Swedish Authority for Privacy Protection (IMY) issues an administrative fine of SEK 7,500,000 against Klarna Bank AB after an investigation has shown that the company has not complied with several of the rules in the GDPR. IMY has now finished an investigation of Klarna Bank AB (Klarna). The authority has examined how the company on its website informs about how it processes personal data in accordance with the GDPR. – Klarna is a financial company that processes personal data about many people and in many different ways. It is important that the information that Klarna provides about how the company processes personal data is correct and as complete as possible. Here we have seen shortcomings, says lawyer Hans Kärnlöf who led the investigation. During the investigation, Klarna has continuously changed the information provided on how the company handles personal data. IMY's decision concerns the information provided in the spring of 2020. In its decision, IMY states that Klarna did not then provide information on the purpose for which and on the basis of which legal basis personal data was processed in one of the company's services. The company also provided incomplete and misleading information about who were the recipients of different categories of personal data when data was shared with Swedish and foreign credit information companies. Klarna also did not provide information on to which countries outside the EU/EEA personal data were transferred or on where and how individuals could obtain information on the safeguards that applied to the transfer to third countries. IMY also notes that the company provided incomplete information about the data subjects' rights, including the right to delete data, the right to data portability and the right to object to how one's personal data is processed. IMY issues an administrative fine against Klarna of SEK 7,500,000 for the deficiencies discovered during the investigation.</t>
+    <t>The Swedish Agency for Privacy Protection (IMY) has reviewed complaints concerning H&amp;M and finds that the company has failed in its handling of requests from individuals who do not want to receive marketing from the company. IMY has initiated a supervision of H&amp;M due to six complaints from individuals who objected to receiving direct marketing from the company. The complaints come from people in Poland, Italy and Great Britain but have been handed over to IMY because H&amp;M has its headquarters in Sweden. – It should be easy to avoid receiving advertising and offers that you are not interested in, says Albin Brunskog who is head of unit at IMY. In its decision, IMY states that H&amp;M has violated the GDPR by not ceasing to handle the complainants' personal data for direct marketing without undue delay, despite the complainants objecting to this. The decision states that the company did not have sufficient systems and routines in place to make it easier for those who complained to exercise their right to object to direct marketing. IMY issues an administrative fine of SEK 350,000 against the company for violations of the GDPR.</t>
   </si>
   <si>
     <t>The Swedish Authority for Privacy Protection (IMY) has investigated the use of camera surveillance at a number of fire stations in Östra Skaraborg and notes that 24/7 surveillance of the staff is too far-reaching. The Swedish Authority for Privacy Protection (IMY) has received information that several fire stations in Östra Skaraborg have surveillance cameras that film spaces where firefighters change clothes in the event of an emergency, and has subsequently initiated an investigation of the camera surveillance. The authority has now completed its investigation and notes that the camera surveillance at the fire stations has been going on in real time around the clock, despite the fact that the Rescue Service in Östra Skaraborg states that the surveillance is only needed when there is an alarm to the fire station in question. – As the camera surveillance has covered employees who are in a dependent relationship to their employer, round-the-clock surveillance is too far-reaching, especially when the Rescue Service states that it is not necessary. In addition, the firefighters have been filmed without any delimitation when they change clothes in the event of an alarm, says Jenny Bård, lawyer at IMY's camera group. IMY states in its decision that the Rescue Service has compelling reasons for its camera surveillance, but that it should be limited so that it is only activated in the event of an alarm and that parts of the area where the fire fighters change clothes should be masked so that only necessary information is captured in the video. The Swedish Authority for Privacy Protection issues an administrative fine of SEK 350,000 against the Executive Board of the Rescue Service in Östra Skaraborg. The camera surveillance has recently ceased.</t>
   </si>
   <si>
-    <t>The Swedish Agency for Privacy Protection (IMY) has reviewed complaints concerning H&amp;M and finds that the company has failed in its handling of requests from individuals who do not want to receive marketing from the company. IMY has initiated a supervision of H&amp;M due to six complaints from individuals who objected to receiving direct marketing from the company. The complaints come from people in Poland, Italy and Great Britain but have been handed over to IMY because H&amp;M has its headquarters in Sweden. – It should be easy to avoid receiving advertising and offers that you are not interested in, says Albin Brunskog who is head of unit at IMY. In its decision, IMY states that H&amp;M has violated the GDPR by not ceasing to handle the complainants' personal data for direct marketing without undue delay, despite the complainants objecting to this. The decision states that the company did not have sufficient systems and routines in place to make it easier for those who complained to exercise their right to object to direct marketing. IMY issues an administrative fine of SEK 350,000 against the company for violations of the GDPR.</t>
-  </si>
-  <si>
-    <t>The Swedish Authority for Privacy Protection (IMY) has audited how four companies use Google Analytics for web statistics. IMY issues administrative fines against two of the companies. One of the companies has recently stopped using the statistics tool on its own initiative, while IMY orders the other three to also stop using it. IMY has audited how four companies transfer personal data to the US via Google Analytics, which is a tool for measuring and analysing traffic on websites. The companies audited are CDON, Coop, Dagens Industri and Tele2. The audits concerns a version of Google Analytics from 14th of August 2020. The audits are based on complaints from the organisation None of Your Business (NOYB) in the light of the Schrems II ruling by the European Court of Justice (CJEU). The complaints allege that the companies, in violation of the law, transfer personal data to the United States. According to the data protection regulation, GDPR, personal data may be transferred to third countries, i.e. countries outside the EU/EEA, if the European Commission has decided that the country in question has an adequate level of protection for personal data that corresponds to that within the EU/EEA. However, the CJEU ruled through the Schrems II ruling that the United States could not be considered to have such an adequate level of protection at the time of the ruling. In its audits, IMY considers that the data transferred to the US via Google's statistics tool is personal data because the data can be linked with other unique data that is transferred. The authority also concludes that the technical security measures that the companies have taken are not sufficient to ensure a level of protection that essentially corresponds to that guaranteed within the EU/EEA. – By the fact that IMY has decided on these cases at the same time, it is made clear what requirements are placed on technical security measures and other measures when transferring personal data to a third country, in this case the United States, says legal advisor Sandra Arvidsson, who led the audits of the companies. If there is no decision on an adequate level of protection by the European Commission, data may be transferred based on standard contractual clauses that the European Commission has decided on. However, according to the CJEU, such standard contractual clauses may need to be supplemented with additional safeguards if it is necessary for the protection that the clauses are intended to provide to be maintained in practice. All four companies have based their decisions on the transfer of personal data via Google Analytics on standard contractual clauses. From IMY's audits, it appears that none of the companies' additional technical security measures are sufficient. IMY issues an administrative fine of 12 million SEK against Tele2 and 300,000 SEK against CDON, which has not taken the same extensive protective measures as Coop and Dagens Industri. Tele2 has recently stopped using the statistics tool on its own initiative. IMY orders the other three companies to stop using the tool. – These decisions have implications not only for these four companies, but can also provide guidance for other organisations that use Google Analytics, says Sandra Arvidsson. Legal advisor Sandra Arvidsson, telephone 08-515 154 14 Press service, telephone 08-515 15 415</t>
-  </si>
-  <si>
-    <t>Swedish Authority for Privacy Protection (DPA) has investigated a co-operative housing association’s use of video surveillance on its property. The DPA concludes that the association has gone too far when using video surveillance in the main entrance and the stairwell and when recording audio. The Swedish DPA has received complaints claiming that a co-operative housing association monitors the stairwell in the association's apartment building. The DPA has now finished an audit of the association. Swedish Authority for Privacy Protection's investigation shows that the association has four surveillance cameras installed. Two are located in the stairwell, one in the main entrance and one is directed towards a distribution box in the association's storage room. All cameras record video and audio non-stop 24 hrs 7 days a week. For the two cameras set up in the stairwell, Swedish Authority for Privacy Protection notes that these allow the association to map the habits, visits and social circle of the residents. "Already the fact that the surveillance is of the residents and their home environment means that it requires very strong reasons for the monitoring to be allowed," writes the authority in its decision. – Under special circumstances, a co-operative housing association may monitor a stairwell. However, in order for such surveillance to be allowed, the association must be able to demonstrate a pressing need for such video surveillance and that has not been the case here, says Nils Henckel, legal advisor at the Swedish DPA. The third camera is set up at the main entrance and the association states that it is to combat problems with vandalism, which it had experienced during two months in 2018. The Swedish DPA stresses the obligation to continuously review whether a need for video surveillance is justified and concludes that no such need was still present to date. As for the fourth camera, which is directed towards the distribution box, the DPA concludes that it must be re-directed so that it does not monitor the residents' storage facilities. Furthermore, Swedish Authority for Privacy Protection notes that audio recording constitutes an additional intrusion into the private sphere, in particular when recorded in a residential building, and that there are no circumstances that motivates such intrusion in this case. The Swedish DPA also concludes that the association has failed to properly inform the residents about the video surveillance. That includes the lack of information about the data controller, where to turn to for further detailed information and that audio is recorded, which is a particularly severe omission. Swedish Authority for Privacy Protection orders the co-operative housing association to stop the video surveillance of the stairwell and entrance, to cease audio recording for the surveillance camera by the distribution box and to improve the information provided concerning the video surveillance. Swedish Authority for Privacy Protection furthermore issues an administrative fine of 20 000 Swedish kronor (approximately 2 000 euro) against the association. When calculating the amount of the fine, consideration was taken to the fact that it was a smaller co-operative housing association</t>
-  </si>
-  <si>
-    <t>The Swedish Authority for Privacy Protection finds that the Swedish Police Authority has processed personal data in breach of the Swedish Criminal Data Act when using Clearview AI to identify individuals. Upon news in the media of the Swedish Police Authority using the application Clearview AI for facial recognition the Swedish Authority for Privacy Protection (IMY) initiated an investigation against the Police. The investigation concludes that Cleaview AI has been used by the Police on a number of occasions. According to the Police a few employees have used the application without any prior authorisation. IMY concludes that the Police has not fulfilled its obligations as a data controller on a number of accounts with regards to the use of Clearview AI. The Police has failed to implement sufficient organisational measures to ensure and be able to demonstrate that the processing of personal data in this case has been carried out in compliance with the Criminal Data Act. When using Clearview AI the Police has unlawfully processed biometric data for facial recognition as well as having failed to conduct a data protection impact assessment which this case of processing would require. – There are clearly defined rules and regulations on how the Police Authority may process personal data, especially for law enforcement purposes. It is the responsibility of the Police to ensure that employees are aware of those rules, says Elena Mazzotti Pallard, legal advisor at IMY. IMY imposes an administrative fine of SEK 2,500,000 (approximately EUR 250,000) on the Police Authority for infringements of the Criminal Data Act. IMY also orders the Police to conduct further training and education of its employees in order to avoid any future processing of personal data in breach of data protection rules and regulations. In addition the Police is ordered to inform the data subjects, whose data has been disclosed to Clearview AI, when confidentiality rules so allows. Finally the Police are ordered to ensure, to the extent possible, that any personal data transferred to Clearview AI is erased.</t>
+    <t>Swedish Authority for Privacy Protection has reviewed the so-called School Platform, the IT system used for, among other things, student administration of schools in the City of Stockholm. The review shows an insufficient level of security of such grave nature that the authority issues an administrative fine of four million SEK against the Board of Education in the City of Stockholm. Swedish Authority for Privacy Protection has received a number of personal data breach notifications from the City of Stockholm's Board of Education. The incidents all relate to the School Platform, which is the IT system used for, among other things, student administration in Stockholm. The school platform contains information of up to 500 000 pupils, guardians and teachers. The system contains sensitive data, including special categories of personal data, as well as information about pupils and teachers with classified information or protected identity. The DPA has reviewed four subsystems in the School Platform and has found serious shortcomings. In one of the subsystems, deficiencies in the ability to restrict users' access to data have allowed large parts of the staff to access information about students with a protected identity. In another subsystem, guardians have been able to access information on other children concerning, for example, grades and evaluations talks in a relatively easy way. Through Google's search engine, it has been possible to find links for login to an administration interface in which information about teachers with a protected identity has been accessible. — In an IT system like this, large amounts of personal data are processed. For such systems it is extremely important that the controller has put in place sufficient security measures in order to protect the data and furthermore to ensure continuous evaluation of the level of protection," says Ranja Bunni, a lawyer at Swedish Authority for Privacy Protection who participated in the investigation. In its decision, Swedish Authority for Privacy Protection finds that the Education Board has not ensured that the personal data in question is processed securely. The Board has failed to take adequate technical and organisational measures to ensure a level of security appropriate in relation to the risk, including a procedure for regularly testing, examining and evaluating the effectiveness of the technical measures in place. Swedish Authority for Privacy Protection issues an administrative fine of four million SEK for the concluded infringements. In Sweden, the maximum amount for administrative fines against public authorities is 10 million SEK. — According to the General Data Protection Regulation, GDPR, administrative fines must be effective, proportional and dissuasive. In this case, the infringements have affected several hundred thousand data subjects, including children and pupils, as well as includes deficiencies in the handling of sensitive and special categories of personal data such as data regarding persons with protected identity and health data, says Salli Fanaei, who also participated in the investigation of Swedish Authority for Privacy Protection.</t>
+  </si>
+  <si>
+    <t>Swedish Authority for Privacy Protection has audited eight health care providers in how they govern and restrict personnel’s access to the main systems for electronic health records. The DPA has discovered insufficiencies that in seven of the eight cases lead to administrative fines of up to SEK 30 million. Swedish Authority for Privacy Protection has now concluded a review of eight health care providers. What has been examined primarily is whether the health care providers have conducted the needs' and risk analysis required in order to assign an adequate access authorisation for personal data in the electronic health records. — Health care providers must carry out a thorough analysis and assessment of the personnel's need to access information in the health records and the risks that accessing patient data includes, according to the Swedish Patient Data Act that is complementary to the GDPR. Without such analysis, health care providers cannot assign the personnel a correct level of authorisation, which in turn means that the organisations cannot guarantee patients' right to privacy protection," says Magnus Bergström, coordinator of the eight audits. Swedish Authority for Privacy Protection notes that seven of the health care providers have not carried out a needs' and risk analysis, while one care provider has carried out an analysis that, however, includes some shortcomings. The authority concludes that seven of the health care providers do not limit the users' access authorisation to the respective patient journal system to what is strictly necessary for the performance of their tasks. — This means that the seven health care providers have not taken appropriate measures to ensure and be able to demonstrate a sufficient level of security for the personal data in the electronic health record systems. The deficiencies of seven healthcare providers are so serious that they result in administrative fines of between SEK 2.5 to 30 million. The calculation of the amount of the fine differs significantly depending on whether it is a private company or a public authority. For companies, the maximum fine is EUR 20 million or four percent of the company's global annual turnover, whichever highest. For authorities, in Sweden the maximum fine is SEK 10 million. Swedish Authority for Privacy Protection has developed guidelines that summarises the conclusions from the audits with regards to the obligation to conduct needs' and risk analyses. — This guidance points to the importance of health care providers ensuring that needs' and risk analyses are carried out. The aim is to help care providers in conducting such analyses, which need to be carried out before any access authorisation is assigned in a health record system. Our hope is now that all the healthcare providers in the country use this guidance in their work to ensure that authorisation is correctly done, in order to guarantee patients the privacy protection they are entitled to, says Magnus Bergström.</t>
   </si>
   <si>
     <t>Umeå University has processed special categories of personal data concerning sexual life and health through, amongst other, storage in a cloud service, without sufficiently protecting the data. Swedish Authority for Privacy Protection is therefore issuing a fine of SEK 550,000 against the university. Swedish Authority for Privacy Protection has now completed an audit of Umeå University, concluding that the University has violated the General Data Protection Regulation by processing special categories of personal data without applying appropriate technical and organisational measures to protect the data. A research group at the University had requested from the police preliminary investigation reports concerning cases of male rape and, upon receiving such reports, proceeded to scanning and storing them digitally. The reports contained information on, among other things, suspicion of crime, name, personal identity number and contact details, as well as sensitive data about sexual life and health. Swedish Authority for Privacy Protection’s investigation shows that the research group stored over a hundred scanned preliminary investigation reports in an American cloud service, despite the University having informed via its intranet that special categories of data should not be stored in the cloud service in question. —The cloud service and the way the university uses it does not provide sufficient protection for this type of personal data, says Linda Hamidi, who led Swedish Authority for Privacy Protection’s audit. When the research group sent an e-mail to the police requesting further information, one of the scanned reports was attached as a reference, a practice that the research group later repeated despite the fact that the police pointed out the inappropriateness in sending sensitive material in unencrypted e-mails. — These events show that the University has not taken necessary measures to ensure a level of security appropriate in relation to the risk. Swedish Authority for Privacy Protection also criticises the University for failing to report the incident as a personal data breach. Since 25 May 2018, organisations are obliged to report personal data breaches to Swedish Authority for Privacy Protection. — The controller is obliged to notify the DPA of data breaches and furthermore to present to us what has been done to mitigate the effects of the incident and to prevent similar incidents from happening in the future. The overall assessment of concluded infringements led to Swedish Authority for Privacy Protection issuing an administrative fine of SEK 550,000 against the University.</t>
   </si>
   <si>
-    <t>The Swedish Authority for Privacy Protection (IMY) has audited how Spotify handles customers' right to access their personal data. The deficiencies that have been discovered cause IMY to issue an administrative fine of SEK 58 million against the company. The General Data Protection Regulation, GDPR, entered into force in 2018 and means, among other things, that the rights of individuals are strengthened. One such right is the right of access, which means a right for individuals to find out what personal data a business handles about the person in question and to receive information about how this data is used. IMY has audited how Spotify handles the right for individuals to access their personal data. IMY assesses that Spotify releases the personal data the company processes when individuals request it, but that the company does not inform clearly enough about how this data is used by the company. - The information that the company provides about how and for what purposes individuals' personal data is handled should be more specific. It must be easy for the person requesting access to their data to understand how the company uses this data. In addition, personal data that is difficult to understand, such as those of a technical nature, may need to be explained not only in English but in the individual's own, native language. In these parts, we have seen certain shortcomings, says Karin Ekström, who is one of the legal advisors who led the supervision. Customers who have turned to Spotify to request access to their personal data have been able to choose which personal data they want access to because Spotify has divided the customers' personal data into different layers. One layer contains the information that Spotify has deemed to be of greatest interest to the individual, for example the customer's contact and payment details, which artists the customer follows and listening history for a certain period of time. If the customer wants more detailed information, for example all technical log files relating to the customer, it has also been possible to request these in another layer. - There is no obstacle to dividing the copy of personal data into different layers as long as the right to access is satisfied. In some situations, on the contrary, it can make it easier for the data subject to take in the information if it is presented in different parts, at least when it is a question of an extensive amount of information. It is important that the individual understands what information is in the various layers and how it can be requested. Here we believe that Spotify has done enough, says Karin Ekström. The purpose of the right of access is to give individuals the opportunity to check that the processing of their personal data is lawful. That the individual receives sufficient information is often a prerequisite for exercising other rights, for example the right to have incorrect information corrected or removed. As the information provided by Spotify has been unclear, it has been difficult for individuals to understand how their personal data is processed and to check whether the handling of their personal data is lawful. Spotify has taken several measures with the aim of meeting the requirements for individuals' right to access, and the deficiencies that have been discovered are considered overall to be of a low level of seriousness. In light of that and, among other things, the number of registered users and Spotify's turnover, IMY issues an administrative fine of SEK 58 million against Spotify for not having provided sufficiently clear information to individuals. Since Spotify has users in many countries, this decision has been made in cooperation with other data protection authorities in the EU.</t>
-  </si>
-  <si>
-    <t>Swedish Authority for Privacy Protection’s investigation shows that the Healthcare Committee in Region Örebro County made a mistake when publishing on the region’s website sensitive personal data about a patient admitted to a forensic psychiatric clinic. Swedish Authority for Privacy Protection received a complaint against the Healthcare Committee in Region Örebro County, in which claims that sensitive personal data about a patient admitted to forensic psychiatry clinic had been published on the region’s website was put forward. – Our investigation into the matter shows that sensitive personal data has wrongfully been published and thereby made accessible to the public on the region’s website", says Elin Hallström, Legal Advisor at Swedish Authority for Privacy Protection. Swedish Authority for Privacy Protection’s audit shows that there are no written instructions relating to the publication of documents and personal data on the website in place. Instructions for publishing information are instead communicated orally. In this case, the instructions had not been followed which led to the accidental publication of the document, suggesting that the Committee had not taken sufficient organizational measures to ensure that personal data is protected from being wrongfully published on the region’s website. – For this reason, we are now ordering the Committee to establish written instructions and introduce measures that ensure that those who publishes personal data on the region’s website does so in accordance with set instructions. In its decision, Swedish Authority for Privacy Protection also concludes that in terms of publication the Committee had neither a legitimate purpose, nor a legal basis, nor fulfilled the requirements for an exemption from the general prohibition against handling sensitive personal data in the General Data Protection Regulation. Swedish Authority for Privacy Protection orders the Committee to bring its personal data handling into compliance and furthermore issues an administrative fine of 120 000 Swedish kronor (approx. 11 000 euro) against the Committee. The published document in question has been removed from the region’s website.</t>
-  </si>
-  <si>
-    <t>Swedish Authority for Privacy Protection has audited eight health care providers in how they govern and restrict personnel’s access to the main systems for electronic health records. The DPA has discovered insufficiencies that in seven of the eight cases lead to administrative fines of up to SEK 30 million. Swedish Authority for Privacy Protection has now concluded a review of eight health care providers. What has been examined primarily is whether the health care providers have conducted the needs' and risk analysis required in order to assign an adequate access authorisation for personal data in the electronic health records. — Health care providers must carry out a thorough analysis and assessment of the personnel's need to access information in the health records and the risks that accessing patient data includes, according to the Swedish Patient Data Act that is complementary to the GDPR. Without such analysis, health care providers cannot assign the personnel a correct level of authorisation, which in turn means that the organisations cannot guarantee patients' right to privacy protection," says Magnus Bergström, coordinator of the eight audits. Swedish Authority for Privacy Protection notes that seven of the health care providers have not carried out a needs' and risk analysis, while one care provider has carried out an analysis that, however, includes some shortcomings. The authority concludes that seven of the health care providers do not limit the users' access authorisation to the respective patient journal system to what is strictly necessary for the performance of their tasks. — This means that the seven health care providers have not taken appropriate measures to ensure and be able to demonstrate a sufficient level of security for the personal data in the electronic health record systems. The deficiencies of seven healthcare providers are so serious that they result in administrative fines of between SEK 2.5 to 30 million. The calculation of the amount of the fine differs significantly depending on whether it is a private company or a public authority. For companies, the maximum fine is EUR 20 million or four percent of the company's global annual turnover, whichever highest. For authorities, in Sweden the maximum fine is SEK 10 million. Swedish Authority for Privacy Protection has developed guidelines that summarises the conclusions from the audits with regards to the obligation to conduct needs' and risk analyses. — This guidance points to the importance of health care providers ensuring that needs' and risk analyses are carried out. The aim is to help care providers in conducting such analyses, which need to be carried out before any access authorisation is assigned in a health record system. Our hope is now that all the healthcare providers in the country use this guidance in their work to ensure that authorisation is correctly done, in order to guarantee patients the privacy protection they are entitled to, says Magnus Bergström.</t>
-  </si>
-  <si>
-    <t>Swedish Authority for Privacy Protection has reviewed the so-called School Platform, the IT system used for, among other things, student administration of schools in the City of Stockholm. The review shows an insufficient level of security of such grave nature that the authority issues an administrative fine of four million SEK against the Board of Education in the City of Stockholm. Swedish Authority for Privacy Protection has received a number of personal data breach notifications from the City of Stockholm's Board of Education. The incidents all relate to the School Platform, which is the IT system used for, among other things, student administration in Stockholm. The school platform contains information of up to 500 000 pupils, guardians and teachers. The system contains sensitive data, including special categories of personal data, as well as information about pupils and teachers with classified information or protected identity. The DPA has reviewed four subsystems in the School Platform and has found serious shortcomings. In one of the subsystems, deficiencies in the ability to restrict users' access to data have allowed large parts of the staff to access information about students with a protected identity. In another subsystem, guardians have been able to access information on other children concerning, for example, grades and evaluations talks in a relatively easy way. Through Google's search engine, it has been possible to find links for login to an administration interface in which information about teachers with a protected identity has been accessible. — In an IT system like this, large amounts of personal data are processed. For such systems it is extremely important that the controller has put in place sufficient security measures in order to protect the data and furthermore to ensure continuous evaluation of the level of protection," says Ranja Bunni, a lawyer at Swedish Authority for Privacy Protection who participated in the investigation. In its decision, Swedish Authority for Privacy Protection finds that the Education Board has not ensured that the personal data in question is processed securely. The Board has failed to take adequate technical and organisational measures to ensure a level of security appropriate in relation to the risk, including a procedure for regularly testing, examining and evaluating the effectiveness of the technical measures in place. Swedish Authority for Privacy Protection issues an administrative fine of four million SEK for the concluded infringements. In Sweden, the maximum amount for administrative fines against public authorities is 10 million SEK. — According to the General Data Protection Regulation, GDPR, administrative fines must be effective, proportional and dissuasive. In this case, the infringements have affected several hundred thousand data subjects, including children and pupils, as well as includes deficiencies in the handling of sensitive and special categories of personal data such as data regarding persons with protected identity and health data, says Salli Fanaei, who also participated in the investigation of Swedish Authority for Privacy Protection.</t>
-  </si>
-  <si>
-    <t>2022-03-30</t>
-  </si>
-  <si>
-    <t>2021-05-27</t>
-  </si>
-  <si>
     <t>2021-05-06</t>
   </si>
   <si>
-    <t>2024-02-22</t>
-  </si>
-  <si>
-    <t>2024-08-14</t>
-  </si>
-  <si>
-    <t>2023-07-04</t>
-  </si>
-  <si>
-    <t>2021-05-26</t>
-  </si>
-  <si>
     <t>2021-05-05</t>
   </si>
   <si>
-    <t>2023-06-14</t>
-  </si>
-  <si>
-    <t>2021-05-07</t>
+    <t>2022-08-30</t>
   </si>
   <si>
     <t>Camera surveillance</t>
   </si>
   <si>
+    <t>Data protection | Internet och appar</t>
+  </si>
+  <si>
     <t>Data protection</t>
   </si>
   <si>
-    <t>Data protection | Internet och appar</t>
+    <t>Data protection | Informationssäkerhet | Personuppgiftsincident</t>
+  </si>
+  <si>
+    <t>Data protection | Dina rättigheter</t>
   </si>
   <si>
     <t>Camera surveillance | Tillsyn</t>
   </si>
   <si>
-    <t>Data protection | Informationssäkerhet | Personuppgiftsincident</t>
-  </si>
-  <si>
-    <t>Data protection | Dina rättigheter</t>
-  </si>
-  <si>
     <t>Data protection | Internet och appar | Brottsbekämpning</t>
   </si>
   <si>
@@ -355,21 +334,21 @@
     <t>https://www.imy.se/en/search-results/?query=Camera%20surveillance</t>
   </si>
   <si>
+    <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Internet%20och%20appar</t>
+  </si>
+  <si>
     <t>https://www.imy.se/en/search-results/?query=Data%20protection</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Internet%20och%20appar</t>
+    <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Informationss%C3%A4kerhet | https://www.imy.se/en/search-results/?query=Personuppgiftsincident</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Dina%20r%C3%A4ttigheter</t>
   </si>
   <si>
     <t>https://www.imy.se/en/search-results/?query=Camera%20surveillance | https://www.imy.se/en/search-results/?query=Tillsyn</t>
   </si>
   <si>
-    <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Informationss%C3%A4kerhet | https://www.imy.se/en/search-results/?query=Personuppgiftsincident</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Dina%20r%C3%A4ttigheter</t>
-  </si>
-  <si>
     <t>https://www.imy.se/en/search-results/?query=Data%20protection | https://www.imy.se/en/search-results/?query=Internet%20och%20appar | https://www.imy.se/en/search-results/?query=Brottsbek%C3%A4mpning</t>
   </si>
   <si>
@@ -385,24 +364,24 @@
     <t>https://www.imy.se/globalassets/dokument/beslut/beslut-tillsyn-gnosjo-2020-11-25.pdf</t>
   </si>
   <si>
+    <t>https://www.imy.se/globalassets/dokument/beslut/2020-03-11-beslut-google.pdf</t>
+  </si>
+  <si>
     <t>https://www.imy.se/globalassets/dokument/beslut/2020-12-14-beslut-tillsyn-uppsalahem.pdf</t>
   </si>
   <si>
-    <t>https://www.imy.se/globalassets/dokument/beslut/2020-03-11-beslut-google.pdf</t>
-  </si>
-  <si>
     <t>https://www.imy.se/globalassets/dokument/beslut/beslut-tillsyn-polismyndigheten-cvai.pdf</t>
   </si>
   <si>
+    <t>https://www.imy.se/globalassets/dokument/beslut/beslut-tillsyn-region-orebro-2020-05-112.pdf</t>
+  </si>
+  <si>
+    <t>https://www.imy.se/globalassets/dokument/beslut/beslut-tillsyn-stockholms-stad.pdf</t>
+  </si>
+  <si>
     <t>https://www.imy.se/globalassets/dokument/beslut/2020-12-10-beslut-tillsyn-umea-universitet.pdf</t>
   </si>
   <si>
-    <t>https://www.imy.se/globalassets/dokument/beslut/beslut-tillsyn-region-orebro-2020-05-112.pdf</t>
-  </si>
-  <si>
-    <t>https://www.imy.se/globalassets/dokument/beslut/beslut-tillsyn-stockholms-stad.pdf</t>
-  </si>
-  <si>
     <t>Legal advisor Elin Hallström | Press officer Per Lövgren</t>
   </si>
   <si>
@@ -415,18 +394,18 @@
     <t>Legal Advisor Elena Mazzotti Pallard | Press Office</t>
   </si>
   <si>
+    <t>Legal Advisor Elin Hallström | Swedish Authority for Privacy Protection’s press office</t>
+  </si>
+  <si>
+    <t>Lawyer Ranja Bunni | Lawyer Salli Fanaei | IT Security Specialist Adolf Slama | Press office</t>
+  </si>
+  <si>
+    <t>Coordinator Magnus Bergström | Press office</t>
+  </si>
+  <si>
     <t>Legal advisor Linda Hamidi | IT security specialist Johan Ma | Press office</t>
   </si>
   <si>
-    <t>Legal Advisor Elin Hallström | Swedish Authority for Privacy Protection’s press office</t>
-  </si>
-  <si>
-    <t>Coordinator Magnus Bergström | Press office</t>
-  </si>
-  <si>
-    <t>Lawyer Ranja Bunni | Lawyer Salli Fanaei | IT Security Specialist Adolf Slama | Press office</t>
-  </si>
-  <si>
     <t>+46-8-657 61 13 | +46-8-515 15　415</t>
   </si>
   <si>
@@ -439,16 +418,16 @@
     <t>+46-8-657 61 72 | +46-8-515 15 415</t>
   </si>
   <si>
+    <t>+46-8-657 61 13 | +46-8-515 15 415</t>
+  </si>
+  <si>
+    <t>+46-8-657 61 46 | +46-8-657 61 45 | +46-8-657 61 12 | +46-8-515 15 415</t>
+  </si>
+  <si>
+    <t>+46-8-657 61 30 | +46-8-515 15 415</t>
+  </si>
+  <si>
     <t>+46-8-657 61 81 | +46-8-657 61 67 | +46-8-515 15 415</t>
-  </si>
-  <si>
-    <t>+46-8-657 61 13 | +46-8-515 15 415</t>
-  </si>
-  <si>
-    <t>+46-8-657 61 30 | +46-8-515 15 415</t>
-  </si>
-  <si>
-    <t>+46-8-657 61 46 | +46-8-657 61 45 | +46-8-657 61 12 | +46-8-515 15 415</t>
   </si>
 </sst>
 </file>
@@ -870,22 +849,22 @@
         <v>73</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L2" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -908,22 +887,22 @@
         <v>74</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J3" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K3" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="L3" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -949,19 +928,19 @@
         <v>93</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="J4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L4" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -984,22 +963,22 @@
         <v>76</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>57</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="K5" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="L5" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1022,22 +1001,22 @@
         <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="I6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" t="s">
         <v>115</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>123</v>
       </c>
-      <c r="K6" t="s">
-        <v>121</v>
-      </c>
       <c r="L6" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1060,22 +1039,22 @@
         <v>78</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" t="s">
         <v>116</v>
       </c>
-      <c r="J7" t="s">
-        <v>121</v>
-      </c>
       <c r="K7" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="L7" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1098,22 +1077,22 @@
         <v>79</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="H8" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="J8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L8" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1136,22 +1115,22 @@
         <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="J9" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="K9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="L9" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1174,22 +1153,22 @@
         <v>81</v>
       </c>
       <c r="G10" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="H10" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I10" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L10" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1197,7 +1176,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>23</v>
@@ -1212,22 +1191,22 @@
         <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="J11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L11" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1244,7 +1223,7 @@
         <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
         <v>83</v>
@@ -1253,19 +1232,19 @@
         <v>93</v>
       </c>
       <c r="H12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="K12" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="L12" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1282,28 +1261,28 @@
         <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F13" t="s">
         <v>84</v>
       </c>
       <c r="G13" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="H13" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="J13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K13" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="L13" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1320,28 +1299,28 @@
         <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F14" t="s">
         <v>85</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="I14" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L14" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1358,28 +1337,28 @@
         <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
         <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="J15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L15" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1387,7 +1366,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
         <v>28</v>
@@ -1396,28 +1375,28 @@
         <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
         <v>87</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="H16" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="I16" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="J16" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="K16" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="L16" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1434,28 +1413,28 @@
         <v>49</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F17" t="s">
         <v>88</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="H17" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="J17" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="K17" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="L17" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1472,28 +1451,28 @@
         <v>50</v>
       </c>
       <c r="E18" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="F18" t="s">
         <v>89</v>
       </c>
       <c r="G18" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="I18" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="L18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1516,22 +1495,22 @@
         <v>90</v>
       </c>
       <c r="G19" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J19" t="s">
+        <v>120</v>
+      </c>
+      <c r="K19" t="s">
         <v>127</v>
       </c>
-      <c r="K19" t="s">
-        <v>134</v>
-      </c>
       <c r="L19" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1554,22 +1533,22 @@
         <v>91</v>
       </c>
       <c r="G20" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H20" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I20" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="J20" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K20" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="L20" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1592,22 +1571,22 @@
         <v>92</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="H21" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I21" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J21" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="K21" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="L21" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>